<commit_message>
remove indices from recipes database xlsx
</commit_message>
<xml_diff>
--- a/recipes.xlsx
+++ b/recipes.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10709"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Firas\Documents\Code\fitdrinks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ll68072/code/other/fitdrinks/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{2314B3BB-810B-034E-BE57-9EC1F6794091}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9885"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All" sheetId="1" r:id="rId1"/>
     <sheet name="With Nutrition Info" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="491">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="573">
   <si>
     <t>Name</t>
   </si>
@@ -1493,12 +1494,258 @@
   </si>
   <si>
     <t>carbs</t>
+  </si>
+  <si>
+    <t>PEANUT BUTTER AND JELLY PROTEIN SMOOTHIE (Serves 1)</t>
+  </si>
+  <si>
+    <t>KEY LIME PIE SHAKE (Serves 1)</t>
+  </si>
+  <si>
+    <t>SKINNY HIGH PROTEIN OREO MILKSHAKE (Serves 2)</t>
+  </si>
+  <si>
+    <t>SUNRISE SMOOTHIE (Serves 1)</t>
+  </si>
+  <si>
+    <t>Dark Chocolate Peppermint Shake (Serves 1)</t>
+  </si>
+  <si>
+    <t>ALMOND BUTTER PROTEIN SMOOTHIE (Serves 1)</t>
+  </si>
+  <si>
+    <t>COFFEE BANANA PROTEIN SMOOTHIE (Serves 3)</t>
+  </si>
+  <si>
+    <t>FRENCH TOAST PROTEIN SHAKE (Serves 1)</t>
+  </si>
+  <si>
+    <t>BERRY OAT SMOOTHIE (Serves 2)</t>
+  </si>
+  <si>
+    <t>ORANGE JULIUS PROTEIN SMOOTHIE (Serves 2)</t>
+  </si>
+  <si>
+    <t>FRESH BLUEBERRY (Serves 1)</t>
+  </si>
+  <si>
+    <t>PEANUT BUTTER CUP (Serves 1)</t>
+  </si>
+  <si>
+    <t>VANILLA CHAI (Serves 1)</t>
+  </si>
+  <si>
+    <t>GREEN MONSTER (Serves 1)</t>
+  </si>
+  <si>
+    <t>COFFEE LOVERS PROTEIN SHAKE (Serves 1)</t>
+  </si>
+  <si>
+    <t>DECADENT VANILLA ALMOND PROTEIN SMOOTHIE (Serves 1)</t>
+  </si>
+  <si>
+    <t>OATMEAL COOKIE PROTEIN SHAKE (Serves 1)</t>
+  </si>
+  <si>
+    <t>OATMEAL RAISIN COOKIE PROTEIN SHAKE (Serves 1)</t>
+  </si>
+  <si>
+    <t>SKINNY APPLE PIE A LA MODE PROTEIN SHAKE (Serves 1)</t>
+  </si>
+  <si>
+    <t>BLUEBERRY PROTEIN SHAKE (Serves 1)</t>
+  </si>
+  <si>
+    <t>SOY ALMOND SHAKE (Serves 1)</t>
+  </si>
+  <si>
+    <t>MOCHA PROTEIN SHAKE (Serves 1)</t>
+  </si>
+  <si>
+    <t>GINGERSNAP PROTEIN SMOOTHIE (Serves 1)</t>
+  </si>
+  <si>
+    <t>APPLE-KALE GREEN SMOOTHIE (Serves 1)</t>
+  </si>
+  <si>
+    <t>BLACK FOREST PROTEIN SHAKE (Serves 1)</t>
+  </si>
+  <si>
+    <t>MANGO BLUEBERRY PROTEIN SMOOTHIE (Serves 1)</t>
+  </si>
+  <si>
+    <t>MANGO LASSI PROTEIN SMOOTHIE (Serves 1)</t>
+  </si>
+  <si>
+    <t>RASPBERRY CHIA PROTEIN SMOOTHIE (Serves 1)</t>
+  </si>
+  <si>
+    <t>TOASTED COCONUT PROTEIN SMOOTHIE (Serves 1)</t>
+  </si>
+  <si>
+    <t>PROTEIN FROSTY SHAKE (Serves 1)</t>
+  </si>
+  <si>
+    <t>BANANA OAT PROTEIN SMOOTHIE (Serves 1)</t>
+  </si>
+  <si>
+    <t>MATCHA PEAR GREEN PROTEIN SMOOTHIE (Serves 1)</t>
+  </si>
+  <si>
+    <t>GRAPE BERRY PROTEIN SHAKE (Serves 1)</t>
+  </si>
+  <si>
+    <t>OATMEAL RAISIN “COOKIE” PROTEIN SMOOTHIE (Serves 1)</t>
+  </si>
+  <si>
+    <t>CHOCOLATE PEANUT BUTTER PROTEIN SHAKE (Serves 1)</t>
+  </si>
+  <si>
+    <t>ORANGE CREAMSICLE PROTEIN SMOOTHIE (Serves 1)</t>
+  </si>
+  <si>
+    <t>WHITE CHOCOLATE RASPBERRY PROTEIN SMOOTHIE (Serves 1)</t>
+  </si>
+  <si>
+    <t>VIETNAMESE COFFEE PROTEIN SMOOTHIE (Serves 1)</t>
+  </si>
+  <si>
+    <t>CINNAMON BANANA BREAD PROTEIN SHAKE (Serves 2)</t>
+  </si>
+  <si>
+    <t>PEANUT BUTTER PROTEIN SHAKE (Serves 2)</t>
+  </si>
+  <si>
+    <t>DARK CHOCOLATE PEPPERMINT PROTEIN SHAKE (Serves 1)</t>
+  </si>
+  <si>
+    <t>CAKE BATTER PROTEIN SHAKE (Serves 2)</t>
+  </si>
+  <si>
+    <t>STRAWBERRY MANGO PROTEIN SHAKE (Serves 3)</t>
+  </si>
+  <si>
+    <t>COFFEE PROTEIN SMOOTHIE (Serves 1)</t>
+  </si>
+  <si>
+    <t>ALOHA BLISS PINEAPPLE PROTEIN SMOOTHIE (Serves 3)</t>
+  </si>
+  <si>
+    <t>BLACKBERRY KIWI PROTEIN SMOOTHIE (Serves 1)</t>
+  </si>
+  <si>
+    <t>MANGO PROTEIN SMOOTHIE (Serves 1)</t>
+  </si>
+  <si>
+    <t>STRAWBERRY WATERMELON PROTEIN SMOOTHIE (Serves 1)</t>
+  </si>
+  <si>
+    <t>PLUM BERRY PROTEIN SMOOTHIE (Serves 2)</t>
+  </si>
+  <si>
+    <t>HONEY &amp; WALNUT SPICED PROTEIN SHAKE (Serves 1)</t>
+  </si>
+  <si>
+    <t>GREEN TEA AVOCADO PROTEIN SMOOTHIE (Serves 1)</t>
+  </si>
+  <si>
+    <t>GINGERBREAD COOKIE PROTEIN SHAKE (Serves 1)</t>
+  </si>
+  <si>
+    <t>APPLE CRUMBLE PROTEIN SMOOTHIE (Serves 2)</t>
+  </si>
+  <si>
+    <t>CHOCOLATE BANANA PROTEIN SHAKE (Serves 1)</t>
+  </si>
+  <si>
+    <t>DARK CHOCOLATE BLUEBERRY PROTEIN SMOOTHIE (Serves 1)</t>
+  </si>
+  <si>
+    <t>STRAWBERRY ORANGE SMOOTHIE (Serves 2 ½ cups)</t>
+  </si>
+  <si>
+    <t>STRAWBERRY BANANA SHAKE</t>
+  </si>
+  <si>
+    <t>DR. MIKE’S POWER SHAKE</t>
+  </si>
+  <si>
+    <t>MANGO TANGO SHAKE</t>
+  </si>
+  <si>
+    <t>PEACH COBBLER PROTEIN SHAKE (Serves 1)</t>
+  </si>
+  <si>
+    <t>BUTTERFINGER PROTEIN SHAKE (Serves 1)</t>
+  </si>
+  <si>
+    <t>STRAWBERRY CHEESECAKE SHAKE (Serves 1)</t>
+  </si>
+  <si>
+    <t>CINNAMON ROLL PROTEIN SHAKE (Serves 1)</t>
+  </si>
+  <si>
+    <t>CHOCOLATE HAZELNUT PROTEIN SHAKE (Serves 1)</t>
+  </si>
+  <si>
+    <t>BLUEBERRY PANCAKE BATTER SMOOTHIE (Serves 1)</t>
+  </si>
+  <si>
+    <t>EARLY MORNING PROTEIN JOLT (Serves 1)</t>
+  </si>
+  <si>
+    <t>AVOCADO MINT PROTEIN SMOOTHIE (Serves 1)</t>
+  </si>
+  <si>
+    <t>BANANA CHAI PROTEIN SHAKE (Serves 1)</t>
+  </si>
+  <si>
+    <t>CHOCOLATE FUDGE PROTEIN SHAKE (Serves 1)</t>
+  </si>
+  <si>
+    <t>LOW CARB CHOCOLATE PROTEIN SHAKE (Serves 1)</t>
+  </si>
+  <si>
+    <t>BLUEBERRY PUMPKIN PIE PROTEIN SHAKE (Serves 1)</t>
+  </si>
+  <si>
+    <t>BEET ORANGE PROTEIN SHAKE (Serves 2)</t>
+  </si>
+  <si>
+    <t>GREEN WARRIOR PROTEIN SMOOTHIE (Serves 2- makes about 3 cups)</t>
+  </si>
+  <si>
+    <t>PINEAPPLE UPSIDE-DOWN CAKE PROTEIN SHAKE (Serves 1)</t>
+  </si>
+  <si>
+    <t>OATMEAL BANANA PROTEIN SHAKE (Serves 1)</t>
+  </si>
+  <si>
+    <t>COCONUT TWISTED JULIUS SMOOTHIE (Serves 1)</t>
+  </si>
+  <si>
+    <t>MUSCULAR MANGO SMOOTHIE (Serves 1)</t>
+  </si>
+  <si>
+    <t>CARAMEL COFFEE SMOOTHIE (Serves 1)</t>
+  </si>
+  <si>
+    <t>THE FUZZY PROTIEN SMOOTHIE (Serves 1)</t>
+  </si>
+  <si>
+    <t>DARK CHOCOLATE BANANA SMOOTHIE (Serves 1)</t>
+  </si>
+  <si>
+    <t>CHOCOLATE PEANUT BUTTER SMOOTHIE (Serves 1)</t>
+  </si>
+  <si>
+    <t>SNICKERS MOCHA SMOOTHIE (Serves 1)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7">
     <font>
       <sz val="10"/>
@@ -1862,18 +2109,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:I251"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="J155" sqref="J155"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="28.5703125" customWidth="1"/>
-    <col min="2" max="2" width="42.85546875" customWidth="1"/>
+    <col min="1" max="1" width="28.5" customWidth="1"/>
+    <col min="2" max="2" width="42.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="13" customFormat="1" ht="15.75" customHeight="1">
@@ -2328,7 +2577,7 @@
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
     </row>
-    <row r="31" spans="1:9" ht="12.75">
+    <row r="31" spans="1:9" ht="13">
       <c r="A31" s="4" t="s">
         <v>94</v>
       </c>
@@ -2343,7 +2592,7 @@
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
     </row>
-    <row r="32" spans="1:9" ht="12.75">
+    <row r="32" spans="1:9" ht="13">
       <c r="A32" s="4" t="s">
         <v>99</v>
       </c>
@@ -2358,7 +2607,7 @@
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
     </row>
-    <row r="33" spans="1:9" ht="12.75">
+    <row r="33" spans="1:9" ht="13">
       <c r="A33" s="4" t="s">
         <v>101</v>
       </c>
@@ -2373,7 +2622,7 @@
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
     </row>
-    <row r="34" spans="1:9" ht="12.75">
+    <row r="34" spans="1:9" ht="13">
       <c r="A34" s="4" t="s">
         <v>103</v>
       </c>
@@ -2388,7 +2637,7 @@
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
     </row>
-    <row r="35" spans="1:9" ht="12.75">
+    <row r="35" spans="1:9" ht="13">
       <c r="A35" s="4" t="s">
         <v>105</v>
       </c>
@@ -2403,7 +2652,7 @@
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
     </row>
-    <row r="36" spans="1:9" ht="12.75">
+    <row r="36" spans="1:9" ht="13">
       <c r="A36" s="4" t="s">
         <v>107</v>
       </c>
@@ -2418,7 +2667,7 @@
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
     </row>
-    <row r="37" spans="1:9" ht="12.75">
+    <row r="37" spans="1:9" ht="13">
       <c r="A37" s="4" t="s">
         <v>110</v>
       </c>
@@ -2433,7 +2682,7 @@
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
     </row>
-    <row r="38" spans="1:9" ht="12.75">
+    <row r="38" spans="1:9" ht="13">
       <c r="A38" s="4" t="s">
         <v>112</v>
       </c>
@@ -2448,7 +2697,7 @@
       <c r="H38" s="2"/>
       <c r="I38" s="2"/>
     </row>
-    <row r="39" spans="1:9" ht="12.75">
+    <row r="39" spans="1:9" ht="13">
       <c r="A39" s="4" t="s">
         <v>115</v>
       </c>
@@ -2463,7 +2712,7 @@
       <c r="H39" s="2"/>
       <c r="I39" s="2"/>
     </row>
-    <row r="40" spans="1:9" ht="12.75">
+    <row r="40" spans="1:9" ht="13">
       <c r="A40" s="4" t="s">
         <v>119</v>
       </c>
@@ -2478,7 +2727,7 @@
       <c r="H40" s="2"/>
       <c r="I40" s="2"/>
     </row>
-    <row r="41" spans="1:9" ht="12.75">
+    <row r="41" spans="1:9" ht="13">
       <c r="A41" s="4" t="s">
         <v>123</v>
       </c>
@@ -2493,7 +2742,7 @@
       <c r="H41" s="4"/>
       <c r="I41" s="4"/>
     </row>
-    <row r="42" spans="1:9" ht="12.75">
+    <row r="42" spans="1:9" ht="13">
       <c r="A42" s="4" t="s">
         <v>127</v>
       </c>
@@ -2508,7 +2757,7 @@
       <c r="H42" s="2"/>
       <c r="I42" s="2"/>
     </row>
-    <row r="43" spans="1:9" ht="12.75">
+    <row r="43" spans="1:9" ht="13">
       <c r="A43" s="4" t="s">
         <v>131</v>
       </c>
@@ -2523,7 +2772,7 @@
       <c r="H43" s="2"/>
       <c r="I43" s="2"/>
     </row>
-    <row r="44" spans="1:9" ht="12.75">
+    <row r="44" spans="1:9" ht="13">
       <c r="A44" s="4" t="s">
         <v>136</v>
       </c>
@@ -2538,7 +2787,7 @@
       <c r="H44" s="2"/>
       <c r="I44" s="2"/>
     </row>
-    <row r="45" spans="1:9" ht="12.75">
+    <row r="45" spans="1:9" ht="13">
       <c r="A45" s="4" t="s">
         <v>140</v>
       </c>
@@ -2553,7 +2802,7 @@
       <c r="H45" s="2"/>
       <c r="I45" s="2"/>
     </row>
-    <row r="46" spans="1:9" ht="12.75">
+    <row r="46" spans="1:9" ht="13">
       <c r="A46" s="4" t="s">
         <v>144</v>
       </c>
@@ -2568,7 +2817,7 @@
       <c r="H46" s="2"/>
       <c r="I46" s="2"/>
     </row>
-    <row r="47" spans="1:9" ht="12.75">
+    <row r="47" spans="1:9" ht="13">
       <c r="A47" s="4" t="s">
         <v>147</v>
       </c>
@@ -2583,7 +2832,7 @@
       <c r="H47" s="2"/>
       <c r="I47" s="2"/>
     </row>
-    <row r="48" spans="1:9" ht="12.75">
+    <row r="48" spans="1:9" ht="13">
       <c r="A48" s="4" t="s">
         <v>151</v>
       </c>
@@ -2598,7 +2847,7 @@
       <c r="H48" s="2"/>
       <c r="I48" s="2"/>
     </row>
-    <row r="49" spans="1:9" ht="12.75">
+    <row r="49" spans="1:9" ht="13">
       <c r="A49" s="4" t="s">
         <v>156</v>
       </c>
@@ -2613,7 +2862,7 @@
       <c r="H49" s="2"/>
       <c r="I49" s="2"/>
     </row>
-    <row r="50" spans="1:9" ht="12.75">
+    <row r="50" spans="1:9" ht="13">
       <c r="A50" s="4" t="s">
         <v>160</v>
       </c>
@@ -2628,7 +2877,7 @@
       <c r="H50" s="2"/>
       <c r="I50" s="2"/>
     </row>
-    <row r="51" spans="1:9" ht="12.75">
+    <row r="51" spans="1:9" ht="13">
       <c r="A51" s="4" t="s">
         <v>123</v>
       </c>
@@ -2643,7 +2892,7 @@
       <c r="H51" s="2"/>
       <c r="I51" s="2"/>
     </row>
-    <row r="52" spans="1:9" ht="12.75">
+    <row r="52" spans="1:9" ht="13">
       <c r="A52" s="4" t="s">
         <v>167</v>
       </c>
@@ -2658,7 +2907,7 @@
       <c r="H52" s="2"/>
       <c r="I52" s="2"/>
     </row>
-    <row r="53" spans="1:9" ht="12.75">
+    <row r="53" spans="1:9" ht="13">
       <c r="A53" s="4" t="s">
         <v>172</v>
       </c>
@@ -2673,7 +2922,7 @@
       <c r="H53" s="2"/>
       <c r="I53" s="2"/>
     </row>
-    <row r="54" spans="1:9" ht="12.75">
+    <row r="54" spans="1:9" ht="13">
       <c r="A54" s="4" t="s">
         <v>182</v>
       </c>
@@ -2688,7 +2937,7 @@
       <c r="H54" s="2"/>
       <c r="I54" s="2"/>
     </row>
-    <row r="55" spans="1:9" ht="12.75">
+    <row r="55" spans="1:9" ht="13">
       <c r="A55" s="4" t="s">
         <v>185</v>
       </c>
@@ -2703,7 +2952,7 @@
       <c r="H55" s="2"/>
       <c r="I55" s="2"/>
     </row>
-    <row r="56" spans="1:9" ht="12.75">
+    <row r="56" spans="1:9" ht="13">
       <c r="A56" s="4" t="s">
         <v>187</v>
       </c>
@@ -2718,7 +2967,7 @@
       <c r="H56" s="2"/>
       <c r="I56" s="2"/>
     </row>
-    <row r="57" spans="1:9" ht="12.75">
+    <row r="57" spans="1:9" ht="13">
       <c r="A57" s="4" t="s">
         <v>167</v>
       </c>
@@ -2733,7 +2982,7 @@
       <c r="H57" s="2"/>
       <c r="I57" s="2"/>
     </row>
-    <row r="58" spans="1:9" ht="12.75">
+    <row r="58" spans="1:9" ht="13">
       <c r="A58" s="10" t="s">
         <v>191</v>
       </c>
@@ -2748,7 +2997,7 @@
       <c r="H58" s="2"/>
       <c r="I58" s="2"/>
     </row>
-    <row r="59" spans="1:9" ht="12.75">
+    <row r="59" spans="1:9" ht="13">
       <c r="A59" s="4" t="s">
         <v>200</v>
       </c>
@@ -2763,7 +3012,7 @@
       <c r="H59" s="2"/>
       <c r="I59" s="2"/>
     </row>
-    <row r="60" spans="1:9" ht="12.75">
+    <row r="60" spans="1:9" ht="13">
       <c r="A60" s="4" t="s">
         <v>204</v>
       </c>
@@ -2778,7 +3027,7 @@
       <c r="H60" s="2"/>
       <c r="I60" s="2"/>
     </row>
-    <row r="61" spans="1:9" ht="12.75">
+    <row r="61" spans="1:9" ht="13">
       <c r="A61" s="4" t="s">
         <v>208</v>
       </c>
@@ -2793,7 +3042,7 @@
       <c r="H61" s="2"/>
       <c r="I61" s="2"/>
     </row>
-    <row r="62" spans="1:9" ht="12.75">
+    <row r="62" spans="1:9" ht="13">
       <c r="A62" s="4" t="s">
         <v>212</v>
       </c>
@@ -2808,7 +3057,7 @@
       <c r="H62" s="2"/>
       <c r="I62" s="2"/>
     </row>
-    <row r="63" spans="1:9" ht="12.75">
+    <row r="63" spans="1:9" ht="13">
       <c r="A63" s="4" t="s">
         <v>217</v>
       </c>
@@ -2823,7 +3072,7 @@
       <c r="H63" s="2"/>
       <c r="I63" s="2"/>
     </row>
-    <row r="64" spans="1:9" ht="12.75">
+    <row r="64" spans="1:9" ht="13">
       <c r="A64" s="4" t="s">
         <v>222</v>
       </c>
@@ -2838,7 +3087,7 @@
       <c r="H64" s="2"/>
       <c r="I64" s="2"/>
     </row>
-    <row r="65" spans="1:9" ht="12.75">
+    <row r="65" spans="1:9" ht="13">
       <c r="A65" s="4" t="s">
         <v>191</v>
       </c>
@@ -2853,7 +3102,7 @@
       <c r="H65" s="2"/>
       <c r="I65" s="2"/>
     </row>
-    <row r="66" spans="1:9" ht="12.75">
+    <row r="66" spans="1:9" ht="13">
       <c r="A66" s="4" t="s">
         <v>229</v>
       </c>
@@ -2868,7 +3117,7 @@
       <c r="H66" s="2"/>
       <c r="I66" s="2"/>
     </row>
-    <row r="67" spans="1:9" ht="12.75">
+    <row r="67" spans="1:9" ht="13">
       <c r="A67" s="4" t="s">
         <v>233</v>
       </c>
@@ -2883,7 +3132,7 @@
       <c r="H67" s="2"/>
       <c r="I67" s="2"/>
     </row>
-    <row r="68" spans="1:9" ht="12.75">
+    <row r="68" spans="1:9" ht="13">
       <c r="A68" s="4" t="s">
         <v>237</v>
       </c>
@@ -2898,7 +3147,7 @@
       <c r="H68" s="2"/>
       <c r="I68" s="2"/>
     </row>
-    <row r="69" spans="1:9" ht="12.75">
+    <row r="69" spans="1:9" ht="13">
       <c r="A69" s="4" t="s">
         <v>241</v>
       </c>
@@ -2913,7 +3162,7 @@
       <c r="H69" s="2"/>
       <c r="I69" s="2"/>
     </row>
-    <row r="70" spans="1:9" ht="12.75">
+    <row r="70" spans="1:9" ht="13">
       <c r="A70" s="4" t="s">
         <v>245</v>
       </c>
@@ -2928,7 +3177,7 @@
       <c r="H70" s="2"/>
       <c r="I70" s="2"/>
     </row>
-    <row r="71" spans="1:9" ht="12.75">
+    <row r="71" spans="1:9" ht="13">
       <c r="A71" s="4" t="s">
         <v>249</v>
       </c>
@@ -2943,7 +3192,7 @@
       <c r="H71" s="2"/>
       <c r="I71" s="2"/>
     </row>
-    <row r="72" spans="1:9" ht="12.75">
+    <row r="72" spans="1:9" ht="13">
       <c r="A72" s="4" t="s">
         <v>254</v>
       </c>
@@ -2958,7 +3207,7 @@
       <c r="H72" s="2"/>
       <c r="I72" s="2"/>
     </row>
-    <row r="73" spans="1:9" ht="12.75">
+    <row r="73" spans="1:9" ht="13">
       <c r="A73" s="4" t="s">
         <v>258</v>
       </c>
@@ -2973,7 +3222,7 @@
       <c r="H73" s="2"/>
       <c r="I73" s="2"/>
     </row>
-    <row r="74" spans="1:9" ht="12.75">
+    <row r="74" spans="1:9" ht="13">
       <c r="A74" s="4" t="s">
         <v>262</v>
       </c>
@@ -2988,7 +3237,7 @@
       <c r="H74" s="2"/>
       <c r="I74" s="2"/>
     </row>
-    <row r="75" spans="1:9" ht="12.75">
+    <row r="75" spans="1:9" ht="13">
       <c r="A75" s="4" t="s">
         <v>267</v>
       </c>
@@ -3003,7 +3252,7 @@
       <c r="H75" s="2"/>
       <c r="I75" s="2"/>
     </row>
-    <row r="76" spans="1:9" ht="12.75">
+    <row r="76" spans="1:9" ht="13">
       <c r="A76" s="4" t="s">
         <v>271</v>
       </c>
@@ -3018,7 +3267,7 @@
       <c r="H76" s="2"/>
       <c r="I76" s="2"/>
     </row>
-    <row r="77" spans="1:9" ht="12.75">
+    <row r="77" spans="1:9" ht="13">
       <c r="A77" s="4" t="s">
         <v>275</v>
       </c>
@@ -3033,7 +3282,7 @@
       <c r="H77" s="2"/>
       <c r="I77" s="2"/>
     </row>
-    <row r="78" spans="1:9" ht="12.75">
+    <row r="78" spans="1:9" ht="13">
       <c r="A78" s="4" t="s">
         <v>279</v>
       </c>
@@ -3048,7 +3297,7 @@
       <c r="H78" s="2"/>
       <c r="I78" s="2"/>
     </row>
-    <row r="79" spans="1:9" ht="12.75">
+    <row r="79" spans="1:9" ht="13">
       <c r="A79" s="4" t="s">
         <v>283</v>
       </c>
@@ -3063,7 +3312,7 @@
       <c r="H79" s="2"/>
       <c r="I79" s="2"/>
     </row>
-    <row r="80" spans="1:9" ht="12.75">
+    <row r="80" spans="1:9" ht="13">
       <c r="A80" s="4" t="s">
         <v>287</v>
       </c>
@@ -3078,7 +3327,7 @@
       <c r="H80" s="2"/>
       <c r="I80" s="2"/>
     </row>
-    <row r="81" spans="1:9" ht="12.75">
+    <row r="81" spans="1:9" ht="13">
       <c r="A81" s="4" t="s">
         <v>291</v>
       </c>
@@ -3093,7 +3342,7 @@
       <c r="H81" s="2"/>
       <c r="I81" s="2"/>
     </row>
-    <row r="82" spans="1:9" ht="12.75">
+    <row r="82" spans="1:9" ht="13">
       <c r="A82" s="4" t="s">
         <v>123</v>
       </c>
@@ -3108,7 +3357,7 @@
       <c r="H82" s="2"/>
       <c r="I82" s="2"/>
     </row>
-    <row r="83" spans="1:9" ht="12.75">
+    <row r="83" spans="1:9" ht="13">
       <c r="A83" s="4" t="s">
         <v>297</v>
       </c>
@@ -3123,7 +3372,7 @@
       <c r="H83" s="2"/>
       <c r="I83" s="2"/>
     </row>
-    <row r="84" spans="1:9" ht="12.75">
+    <row r="84" spans="1:9" ht="13">
       <c r="A84" s="4" t="s">
         <v>301</v>
       </c>
@@ -3138,7 +3387,7 @@
       <c r="H84" s="2"/>
       <c r="I84" s="2"/>
     </row>
-    <row r="85" spans="1:9" ht="12.75">
+    <row r="85" spans="1:9" ht="13">
       <c r="A85" s="4" t="s">
         <v>123</v>
       </c>
@@ -3153,7 +3402,7 @@
       <c r="H85" s="2"/>
       <c r="I85" s="2"/>
     </row>
-    <row r="86" spans="1:9" ht="12.75">
+    <row r="86" spans="1:9" ht="13">
       <c r="A86" s="4" t="s">
         <v>309</v>
       </c>
@@ -3168,7 +3417,7 @@
       <c r="H86" s="2"/>
       <c r="I86" s="2"/>
     </row>
-    <row r="87" spans="1:9" ht="12.75">
+    <row r="87" spans="1:9" ht="13">
       <c r="A87" s="4" t="s">
         <v>123</v>
       </c>
@@ -3183,7 +3432,7 @@
       <c r="H87" s="2"/>
       <c r="I87" s="2"/>
     </row>
-    <row r="88" spans="1:9" ht="12.75">
+    <row r="88" spans="1:9" ht="13">
       <c r="A88" s="4" t="s">
         <v>318</v>
       </c>
@@ -3198,7 +3447,7 @@
       <c r="H88" s="2"/>
       <c r="I88" s="2"/>
     </row>
-    <row r="89" spans="1:9" ht="12.75">
+    <row r="89" spans="1:9" ht="13">
       <c r="A89" s="4" t="s">
         <v>322</v>
       </c>
@@ -3213,7 +3462,7 @@
       <c r="H89" s="2"/>
       <c r="I89" s="2"/>
     </row>
-    <row r="90" spans="1:9" ht="12.75">
+    <row r="90" spans="1:9" ht="13">
       <c r="A90" s="4" t="s">
         <v>326</v>
       </c>
@@ -3228,7 +3477,7 @@
       <c r="H90" s="2"/>
       <c r="I90" s="2"/>
     </row>
-    <row r="91" spans="1:9" ht="12.75">
+    <row r="91" spans="1:9" ht="13">
       <c r="A91" s="4" t="s">
         <v>330</v>
       </c>
@@ -3243,7 +3492,7 @@
       <c r="H91" s="2"/>
       <c r="I91" s="2"/>
     </row>
-    <row r="92" spans="1:9" ht="12.75">
+    <row r="92" spans="1:9" ht="13">
       <c r="A92" s="4" t="s">
         <v>334</v>
       </c>
@@ -3258,7 +3507,7 @@
       <c r="H92" s="2"/>
       <c r="I92" s="2"/>
     </row>
-    <row r="93" spans="1:9" ht="12.75">
+    <row r="93" spans="1:9" ht="13">
       <c r="A93" s="4" t="s">
         <v>339</v>
       </c>
@@ -3273,7 +3522,7 @@
       <c r="H93" s="2"/>
       <c r="I93" s="2"/>
     </row>
-    <row r="94" spans="1:9" ht="12.75">
+    <row r="94" spans="1:9" ht="13">
       <c r="A94" s="4" t="s">
         <v>343</v>
       </c>
@@ -3288,7 +3537,7 @@
       <c r="H94" s="2"/>
       <c r="I94" s="2"/>
     </row>
-    <row r="95" spans="1:9" ht="12.75">
+    <row r="95" spans="1:9" ht="13">
       <c r="A95" s="4" t="s">
         <v>347</v>
       </c>
@@ -3303,7 +3552,7 @@
       <c r="H95" s="2"/>
       <c r="I95" s="2"/>
     </row>
-    <row r="96" spans="1:9" ht="12.75">
+    <row r="96" spans="1:9" ht="13">
       <c r="A96" s="4" t="s">
         <v>350</v>
       </c>
@@ -3318,7 +3567,7 @@
       <c r="H96" s="2"/>
       <c r="I96" s="2"/>
     </row>
-    <row r="97" spans="1:9" ht="12.75">
+    <row r="97" spans="1:9" ht="13">
       <c r="A97" s="4" t="s">
         <v>352</v>
       </c>
@@ -3333,7 +3582,7 @@
       <c r="H97" s="2"/>
       <c r="I97" s="2"/>
     </row>
-    <row r="98" spans="1:9" ht="12.75">
+    <row r="98" spans="1:9" ht="13">
       <c r="A98" s="4" t="s">
         <v>354</v>
       </c>
@@ -3348,7 +3597,7 @@
       <c r="H98" s="2"/>
       <c r="I98" s="2"/>
     </row>
-    <row r="99" spans="1:9" ht="12.75">
+    <row r="99" spans="1:9" ht="13">
       <c r="A99" s="4" t="s">
         <v>356</v>
       </c>
@@ -3363,7 +3612,7 @@
       <c r="H99" s="2"/>
       <c r="I99" s="2"/>
     </row>
-    <row r="100" spans="1:9" ht="12.75">
+    <row r="100" spans="1:9" ht="13">
       <c r="A100" s="4" t="s">
         <v>361</v>
       </c>
@@ -3378,7 +3627,7 @@
       <c r="H100" s="2"/>
       <c r="I100" s="2"/>
     </row>
-    <row r="101" spans="1:9" ht="12.75">
+    <row r="101" spans="1:9" ht="13">
       <c r="A101" s="4" t="s">
         <v>366</v>
       </c>
@@ -3393,7 +3642,7 @@
       <c r="H101" s="2"/>
       <c r="I101" s="2"/>
     </row>
-    <row r="102" spans="1:9" ht="12.75">
+    <row r="102" spans="1:9" ht="13">
       <c r="A102" s="4" t="s">
         <v>370</v>
       </c>
@@ -3408,7 +3657,7 @@
       <c r="H102" s="2"/>
       <c r="I102" s="2"/>
     </row>
-    <row r="103" spans="1:9" ht="12.75">
+    <row r="103" spans="1:9" ht="13">
       <c r="A103" s="4" t="s">
         <v>373</v>
       </c>
@@ -3423,7 +3672,7 @@
       <c r="H103" s="2"/>
       <c r="I103" s="2"/>
     </row>
-    <row r="104" spans="1:9" ht="12.75">
+    <row r="104" spans="1:9" ht="13">
       <c r="A104" s="4" t="s">
         <v>376</v>
       </c>
@@ -3438,7 +3687,7 @@
       <c r="H104" s="2"/>
       <c r="I104" s="2"/>
     </row>
-    <row r="105" spans="1:9" ht="12.75">
+    <row r="105" spans="1:9" ht="13">
       <c r="A105" s="4" t="s">
         <v>151</v>
       </c>
@@ -3453,7 +3702,7 @@
       <c r="H105" s="2"/>
       <c r="I105" s="2"/>
     </row>
-    <row r="106" spans="1:9" ht="12.75">
+    <row r="106" spans="1:9" ht="13">
       <c r="A106" s="4" t="s">
         <v>384</v>
       </c>
@@ -3468,7 +3717,7 @@
       <c r="H106" s="2"/>
       <c r="I106" s="2"/>
     </row>
-    <row r="107" spans="1:9" ht="12.75">
+    <row r="107" spans="1:9" ht="13">
       <c r="A107" s="4" t="s">
         <v>356</v>
       </c>
@@ -3483,7 +3732,7 @@
       <c r="H107" s="2"/>
       <c r="I107" s="2"/>
     </row>
-    <row r="108" spans="1:9" ht="12.75">
+    <row r="108" spans="1:9" ht="13">
       <c r="A108" s="4" t="s">
         <v>392</v>
       </c>
@@ -3498,7 +3747,7 @@
       <c r="H108" s="2"/>
       <c r="I108" s="2"/>
     </row>
-    <row r="109" spans="1:9" ht="12.75">
+    <row r="109" spans="1:9" ht="13">
       <c r="A109" s="4" t="s">
         <v>397</v>
       </c>
@@ -3513,7 +3762,7 @@
       <c r="H109" s="2"/>
       <c r="I109" s="2"/>
     </row>
-    <row r="110" spans="1:9" ht="12.75">
+    <row r="110" spans="1:9" ht="13">
       <c r="A110" s="4" t="s">
         <v>361</v>
       </c>
@@ -3528,7 +3777,7 @@
       <c r="H110" s="2"/>
       <c r="I110" s="2"/>
     </row>
-    <row r="111" spans="1:9" ht="12.75">
+    <row r="111" spans="1:9" ht="13">
       <c r="A111" s="4" t="s">
         <v>403</v>
       </c>
@@ -3543,7 +3792,7 @@
       <c r="H111" s="2"/>
       <c r="I111" s="2"/>
     </row>
-    <row r="112" spans="1:9" ht="12.75">
+    <row r="112" spans="1:9" ht="13">
       <c r="A112" s="4" t="s">
         <v>330</v>
       </c>
@@ -3558,7 +3807,7 @@
       <c r="H112" s="2"/>
       <c r="I112" s="2"/>
     </row>
-    <row r="113" spans="1:9" ht="12.75">
+    <row r="113" spans="1:9" ht="13">
       <c r="A113" s="4" t="s">
         <v>410</v>
       </c>
@@ -3573,7 +3822,7 @@
       <c r="H113" s="2"/>
       <c r="I113" s="2"/>
     </row>
-    <row r="114" spans="1:9" ht="12.75">
+    <row r="114" spans="1:9" ht="13">
       <c r="A114" s="4" t="s">
         <v>347</v>
       </c>
@@ -3588,7 +3837,7 @@
       <c r="H114" s="2"/>
       <c r="I114" s="2"/>
     </row>
-    <row r="115" spans="1:9" ht="12.75">
+    <row r="115" spans="1:9" ht="13">
       <c r="A115" s="4" t="s">
         <v>297</v>
       </c>
@@ -3603,7 +3852,7 @@
       <c r="H115" s="2"/>
       <c r="I115" s="2"/>
     </row>
-    <row r="116" spans="1:9" ht="12.75">
+    <row r="116" spans="1:9" ht="13">
       <c r="A116" s="4" t="s">
         <v>415</v>
       </c>
@@ -3618,7 +3867,7 @@
       <c r="H116" s="2"/>
       <c r="I116" s="2"/>
     </row>
-    <row r="117" spans="1:9" ht="12.75">
+    <row r="117" spans="1:9" ht="13">
       <c r="A117" s="4" t="s">
         <v>417</v>
       </c>
@@ -3633,7 +3882,7 @@
       <c r="H117" s="2"/>
       <c r="I117" s="2"/>
     </row>
-    <row r="118" spans="1:9" ht="12.75">
+    <row r="118" spans="1:9" ht="13">
       <c r="A118" s="4" t="s">
         <v>419</v>
       </c>
@@ -3648,7 +3897,7 @@
       <c r="H118" s="2"/>
       <c r="I118" s="2"/>
     </row>
-    <row r="119" spans="1:9" ht="12.75">
+    <row r="119" spans="1:9" ht="13">
       <c r="A119" s="4" t="s">
         <v>421</v>
       </c>
@@ -3663,7 +3912,7 @@
       <c r="H119" s="2"/>
       <c r="I119" s="2"/>
     </row>
-    <row r="120" spans="1:9" ht="12.75">
+    <row r="120" spans="1:9" ht="13">
       <c r="A120" s="4" t="s">
         <v>423</v>
       </c>
@@ -3678,7 +3927,7 @@
       <c r="H120" s="2"/>
       <c r="I120" s="2"/>
     </row>
-    <row r="121" spans="1:9" ht="12.75">
+    <row r="121" spans="1:9" ht="13">
       <c r="A121" s="4" t="s">
         <v>425</v>
       </c>
@@ -3693,7 +3942,7 @@
       <c r="H121" s="2"/>
       <c r="I121" s="2"/>
     </row>
-    <row r="122" spans="1:9" ht="12.75">
+    <row r="122" spans="1:9" ht="13">
       <c r="A122" s="4" t="s">
         <v>427</v>
       </c>
@@ -3708,7 +3957,7 @@
       <c r="H122" s="2"/>
       <c r="I122" s="2"/>
     </row>
-    <row r="123" spans="1:9" ht="12.75">
+    <row r="123" spans="1:9" ht="13">
       <c r="A123" s="4" t="s">
         <v>429</v>
       </c>
@@ -3723,7 +3972,7 @@
       <c r="H123" s="2"/>
       <c r="I123" s="2"/>
     </row>
-    <row r="124" spans="1:9" ht="12.75">
+    <row r="124" spans="1:9" ht="13">
       <c r="A124" s="4" t="s">
         <v>431</v>
       </c>
@@ -3738,7 +3987,7 @@
       <c r="H124" s="2"/>
       <c r="I124" s="2"/>
     </row>
-    <row r="125" spans="1:9" ht="12.75">
+    <row r="125" spans="1:9" ht="13">
       <c r="A125" s="4" t="s">
         <v>433</v>
       </c>
@@ -3753,7 +4002,7 @@
       <c r="H125" s="2"/>
       <c r="I125" s="2"/>
     </row>
-    <row r="126" spans="1:9" ht="12.75">
+    <row r="126" spans="1:9" ht="13">
       <c r="A126" s="4" t="s">
         <v>435</v>
       </c>
@@ -3768,7 +4017,7 @@
       <c r="H126" s="2"/>
       <c r="I126" s="2"/>
     </row>
-    <row r="127" spans="1:9" ht="12.75">
+    <row r="127" spans="1:9" ht="13">
       <c r="A127" s="4" t="s">
         <v>437</v>
       </c>
@@ -3783,7 +4032,7 @@
       <c r="H127" s="2"/>
       <c r="I127" s="2"/>
     </row>
-    <row r="128" spans="1:9" ht="12.75">
+    <row r="128" spans="1:9" ht="13">
       <c r="A128" s="4" t="s">
         <v>439</v>
       </c>
@@ -3798,7 +4047,7 @@
       <c r="H128" s="2"/>
       <c r="I128" s="2"/>
     </row>
-    <row r="129" spans="1:9" ht="12.75">
+    <row r="129" spans="1:9" ht="13">
       <c r="A129" s="4" t="s">
         <v>441</v>
       </c>
@@ -3813,7 +4062,7 @@
       <c r="H129" s="2"/>
       <c r="I129" s="2"/>
     </row>
-    <row r="130" spans="1:9" ht="12.75">
+    <row r="130" spans="1:9" ht="13">
       <c r="A130" s="4" t="s">
         <v>443</v>
       </c>
@@ -3828,7 +4077,7 @@
       <c r="H130" s="2"/>
       <c r="I130" s="2"/>
     </row>
-    <row r="131" spans="1:9" ht="12.75">
+    <row r="131" spans="1:9" ht="13">
       <c r="A131" s="4" t="s">
         <v>445</v>
       </c>
@@ -3843,7 +4092,7 @@
       <c r="H131" s="2"/>
       <c r="I131" s="2"/>
     </row>
-    <row r="132" spans="1:9" ht="12.75">
+    <row r="132" spans="1:9" ht="13">
       <c r="A132" s="4" t="s">
         <v>447</v>
       </c>
@@ -3858,7 +4107,7 @@
       <c r="H132" s="2"/>
       <c r="I132" s="2"/>
     </row>
-    <row r="133" spans="1:9" ht="12.75">
+    <row r="133" spans="1:9" ht="13">
       <c r="A133" s="4" t="s">
         <v>449</v>
       </c>
@@ -3873,7 +4122,7 @@
       <c r="H133" s="2"/>
       <c r="I133" s="2"/>
     </row>
-    <row r="134" spans="1:9" ht="12.75">
+    <row r="134" spans="1:9" ht="13">
       <c r="A134" s="4" t="s">
         <v>451</v>
       </c>
@@ -3888,7 +4137,7 @@
       <c r="H134" s="2"/>
       <c r="I134" s="2"/>
     </row>
-    <row r="135" spans="1:9" ht="12.75">
+    <row r="135" spans="1:9" ht="13">
       <c r="A135" s="4" t="s">
         <v>453</v>
       </c>
@@ -3903,7 +4152,7 @@
       <c r="H135" s="2"/>
       <c r="I135" s="2"/>
     </row>
-    <row r="136" spans="1:9" ht="12.75">
+    <row r="136" spans="1:9" ht="13">
       <c r="A136" s="4" t="s">
         <v>455</v>
       </c>
@@ -3918,7 +4167,7 @@
       <c r="H136" s="2"/>
       <c r="I136" s="2"/>
     </row>
-    <row r="137" spans="1:9" ht="12.75">
+    <row r="137" spans="1:9" ht="13">
       <c r="A137" s="4" t="s">
         <v>457</v>
       </c>
@@ -3933,7 +4182,7 @@
       <c r="H137" s="2"/>
       <c r="I137" s="2"/>
     </row>
-    <row r="138" spans="1:9" ht="12.75">
+    <row r="138" spans="1:9" ht="13">
       <c r="A138" s="4" t="s">
         <v>459</v>
       </c>
@@ -3948,7 +4197,7 @@
       <c r="H138" s="2"/>
       <c r="I138" s="2"/>
     </row>
-    <row r="139" spans="1:9" ht="12.75">
+    <row r="139" spans="1:9" ht="13">
       <c r="A139" s="4" t="s">
         <v>461</v>
       </c>
@@ -3963,7 +4212,7 @@
       <c r="H139" s="2"/>
       <c r="I139" s="2"/>
     </row>
-    <row r="140" spans="1:9" ht="12.75">
+    <row r="140" spans="1:9" ht="13">
       <c r="A140" s="4" t="s">
         <v>463</v>
       </c>
@@ -3978,7 +4227,7 @@
       <c r="H140" s="2"/>
       <c r="I140" s="2"/>
     </row>
-    <row r="141" spans="1:9" ht="12.75">
+    <row r="141" spans="1:9" ht="13">
       <c r="A141" s="4" t="s">
         <v>465</v>
       </c>
@@ -3993,7 +4242,7 @@
       <c r="H141" s="2"/>
       <c r="I141" s="2"/>
     </row>
-    <row r="142" spans="1:9" ht="12.75">
+    <row r="142" spans="1:9" ht="13">
       <c r="A142" s="4" t="s">
         <v>467</v>
       </c>
@@ -4008,7 +4257,7 @@
       <c r="H142" s="2"/>
       <c r="I142" s="2"/>
     </row>
-    <row r="143" spans="1:9" ht="12.75">
+    <row r="143" spans="1:9" ht="13">
       <c r="A143" s="4" t="s">
         <v>469</v>
       </c>
@@ -4023,7 +4272,7 @@
       <c r="H143" s="2"/>
       <c r="I143" s="2"/>
     </row>
-    <row r="144" spans="1:9" ht="12.75">
+    <row r="144" spans="1:9" ht="13">
       <c r="A144" s="4" t="s">
         <v>471</v>
       </c>
@@ -4038,7 +4287,7 @@
       <c r="H144" s="2"/>
       <c r="I144" s="2"/>
     </row>
-    <row r="145" spans="1:9" ht="12.75">
+    <row r="145" spans="1:9" ht="13">
       <c r="A145" s="4" t="s">
         <v>473</v>
       </c>
@@ -4053,7 +4302,7 @@
       <c r="H145" s="2"/>
       <c r="I145" s="2"/>
     </row>
-    <row r="146" spans="1:9" ht="12.75">
+    <row r="146" spans="1:9" ht="13">
       <c r="A146" s="4" t="s">
         <v>475</v>
       </c>
@@ -4068,7 +4317,7 @@
       <c r="H146" s="2"/>
       <c r="I146" s="2"/>
     </row>
-    <row r="147" spans="1:9" ht="12.75">
+    <row r="147" spans="1:9" ht="13">
       <c r="A147" s="4" t="s">
         <v>477</v>
       </c>
@@ -4083,7 +4332,7 @@
       <c r="H147" s="2"/>
       <c r="I147" s="2"/>
     </row>
-    <row r="148" spans="1:9" ht="12.75">
+    <row r="148" spans="1:9" ht="13">
       <c r="A148" s="4" t="s">
         <v>469</v>
       </c>
@@ -4098,7 +4347,7 @@
       <c r="H148" s="2"/>
       <c r="I148" s="2"/>
     </row>
-    <row r="149" spans="1:9" ht="12.75">
+    <row r="149" spans="1:9" ht="13">
       <c r="A149" s="4" t="s">
         <v>480</v>
       </c>
@@ -4113,7 +4362,7 @@
       <c r="H149" s="2"/>
       <c r="I149" s="2"/>
     </row>
-    <row r="150" spans="1:9" ht="12.75">
+    <row r="150" spans="1:9" ht="13">
       <c r="A150" s="4" t="s">
         <v>482</v>
       </c>
@@ -4128,7 +4377,7 @@
       <c r="H150" s="2"/>
       <c r="I150" s="2"/>
     </row>
-    <row r="151" spans="1:9" ht="12.75">
+    <row r="151" spans="1:9" ht="13">
       <c r="A151" s="4" t="s">
         <v>484</v>
       </c>
@@ -4145,7 +4394,7 @@
     </row>
     <row r="152" spans="1:9" ht="15">
       <c r="A152" s="6" t="s">
-        <v>11</v>
+        <v>491</v>
       </c>
       <c r="B152" s="6" t="s">
         <v>21</v>
@@ -4160,13 +4409,13 @@
         <v>23</v>
       </c>
       <c r="F152" s="2"/>
-      <c r="G152" s="2"/>
+      <c r="G152" s="7"/>
       <c r="H152" s="2"/>
       <c r="I152" s="2"/>
     </row>
     <row r="153" spans="1:9" ht="15">
       <c r="A153" s="6" t="s">
-        <v>27</v>
+        <v>492</v>
       </c>
       <c r="B153" s="6" t="s">
         <v>30</v>
@@ -4181,13 +4430,13 @@
         <v>17</v>
       </c>
       <c r="F153" s="2"/>
-      <c r="G153" s="2"/>
+      <c r="G153" s="7"/>
       <c r="H153" s="2"/>
       <c r="I153" s="2"/>
     </row>
     <row r="154" spans="1:9" ht="15">
       <c r="A154" s="6" t="s">
-        <v>32</v>
+        <v>493</v>
       </c>
       <c r="B154" s="6" t="s">
         <v>34</v>
@@ -4202,13 +4451,13 @@
         <v>24</v>
       </c>
       <c r="F154" s="2"/>
-      <c r="G154" s="2"/>
+      <c r="G154" s="7"/>
       <c r="H154" s="2"/>
       <c r="I154" s="2"/>
     </row>
     <row r="155" spans="1:9" ht="15">
       <c r="A155" s="6" t="s">
-        <v>36</v>
+        <v>494</v>
       </c>
       <c r="B155" s="6" t="s">
         <v>38</v>
@@ -4223,13 +4472,13 @@
         <v>42</v>
       </c>
       <c r="F155" s="2"/>
-      <c r="G155" s="2"/>
+      <c r="G155" s="7"/>
       <c r="H155" s="2"/>
       <c r="I155" s="2"/>
     </row>
     <row r="156" spans="1:9" ht="15">
       <c r="A156" s="6" t="s">
-        <v>45</v>
+        <v>495</v>
       </c>
       <c r="B156" s="6" t="s">
         <v>46</v>
@@ -4244,13 +4493,13 @@
         <v>20</v>
       </c>
       <c r="F156" s="2"/>
-      <c r="G156" s="2"/>
+      <c r="G156" s="7"/>
       <c r="H156" s="2"/>
       <c r="I156" s="2"/>
     </row>
     <row r="157" spans="1:9" ht="15">
       <c r="A157" s="6" t="s">
-        <v>48</v>
+        <v>496</v>
       </c>
       <c r="B157" s="6" t="s">
         <v>50</v>
@@ -4265,13 +4514,13 @@
         <v>39</v>
       </c>
       <c r="F157" s="2"/>
-      <c r="G157" s="2"/>
+      <c r="G157" s="7"/>
       <c r="H157" s="2"/>
       <c r="I157" s="2"/>
     </row>
     <row r="158" spans="1:9" ht="15">
       <c r="A158" s="6" t="s">
-        <v>52</v>
+        <v>497</v>
       </c>
       <c r="B158" s="6" t="s">
         <v>54</v>
@@ -4286,13 +4535,13 @@
         <v>25</v>
       </c>
       <c r="F158" s="2"/>
-      <c r="G158" s="2"/>
+      <c r="G158" s="7"/>
       <c r="H158" s="2"/>
       <c r="I158" s="2"/>
     </row>
     <row r="159" spans="1:9" ht="15">
       <c r="A159" s="6" t="s">
-        <v>57</v>
+        <v>498</v>
       </c>
       <c r="B159" s="6" t="s">
         <v>60</v>
@@ -4307,13 +4556,13 @@
         <v>12</v>
       </c>
       <c r="F159" s="2"/>
-      <c r="G159" s="2"/>
+      <c r="G159" s="7"/>
       <c r="H159" s="2"/>
       <c r="I159" s="2"/>
     </row>
     <row r="160" spans="1:9" ht="15">
       <c r="A160" s="6" t="s">
-        <v>65</v>
+        <v>499</v>
       </c>
       <c r="B160" s="6" t="s">
         <v>66</v>
@@ -4328,13 +4577,13 @@
         <v>56.6</v>
       </c>
       <c r="F160" s="2"/>
-      <c r="G160" s="2"/>
+      <c r="G160" s="7"/>
       <c r="H160" s="2"/>
       <c r="I160" s="2"/>
     </row>
     <row r="161" spans="1:9" ht="15">
       <c r="A161" s="6" t="s">
-        <v>67</v>
+        <v>500</v>
       </c>
       <c r="B161" s="6" t="s">
         <v>68</v>
@@ -4355,7 +4604,7 @@
     </row>
     <row r="162" spans="1:9" ht="15">
       <c r="A162" s="6" t="s">
-        <v>69</v>
+        <v>501</v>
       </c>
       <c r="B162" s="6" t="s">
         <v>70</v>
@@ -4370,13 +4619,13 @@
         <v>16</v>
       </c>
       <c r="F162" s="2"/>
-      <c r="G162" s="2"/>
+      <c r="G162" s="7"/>
       <c r="H162" s="2"/>
       <c r="I162" s="2"/>
     </row>
     <row r="163" spans="1:9" ht="15">
       <c r="A163" s="6" t="s">
-        <v>71</v>
+        <v>502</v>
       </c>
       <c r="B163" s="6" t="s">
         <v>73</v>
@@ -4391,13 +4640,13 @@
         <v>21</v>
       </c>
       <c r="F163" s="2"/>
-      <c r="G163" s="2"/>
+      <c r="G163" s="7"/>
       <c r="H163" s="2"/>
       <c r="I163" s="2"/>
     </row>
     <row r="164" spans="1:9" ht="15">
       <c r="A164" s="6" t="s">
-        <v>74</v>
+        <v>503</v>
       </c>
       <c r="B164" s="6" t="s">
         <v>76</v>
@@ -4412,13 +4661,13 @@
         <v>20</v>
       </c>
       <c r="F164" s="2"/>
-      <c r="G164" s="2"/>
+      <c r="G164" s="7"/>
       <c r="H164" s="2"/>
       <c r="I164" s="2"/>
     </row>
     <row r="165" spans="1:9" ht="15">
       <c r="A165" s="6" t="s">
-        <v>78</v>
+        <v>504</v>
       </c>
       <c r="B165" s="6" t="s">
         <v>80</v>
@@ -4433,13 +4682,13 @@
         <v>40</v>
       </c>
       <c r="F165" s="2"/>
-      <c r="G165" s="2"/>
+      <c r="G165" s="7"/>
       <c r="H165" s="2"/>
       <c r="I165" s="2"/>
     </row>
     <row r="166" spans="1:9" ht="15">
       <c r="A166" s="6" t="s">
-        <v>82</v>
+        <v>505</v>
       </c>
       <c r="B166" s="6" t="s">
         <v>84</v>
@@ -4454,13 +4703,13 @@
         <v>19</v>
       </c>
       <c r="F166" s="2"/>
-      <c r="G166" s="2"/>
+      <c r="G166" s="7"/>
       <c r="H166" s="2"/>
       <c r="I166" s="2"/>
     </row>
     <row r="167" spans="1:9" ht="15">
       <c r="A167" s="6" t="s">
-        <v>87</v>
+        <v>506</v>
       </c>
       <c r="B167" s="6" t="s">
         <v>89</v>
@@ -4475,13 +4724,13 @@
         <v>28</v>
       </c>
       <c r="F167" s="2"/>
-      <c r="G167" s="2"/>
+      <c r="G167" s="7"/>
       <c r="H167" s="2"/>
       <c r="I167" s="2"/>
     </row>
     <row r="168" spans="1:9" ht="15">
       <c r="A168" s="6" t="s">
-        <v>91</v>
+        <v>507</v>
       </c>
       <c r="B168" s="6" t="s">
         <v>93</v>
@@ -4496,13 +4745,13 @@
         <v>21</v>
       </c>
       <c r="F168" s="2"/>
-      <c r="G168" s="2"/>
+      <c r="G168" s="7"/>
       <c r="H168" s="2"/>
       <c r="I168" s="2"/>
     </row>
     <row r="169" spans="1:9" ht="15">
       <c r="A169" s="6" t="s">
-        <v>95</v>
+        <v>508</v>
       </c>
       <c r="B169" s="6" t="s">
         <v>96</v>
@@ -4517,13 +4766,13 @@
         <v>35</v>
       </c>
       <c r="F169" s="2"/>
-      <c r="G169" s="2"/>
+      <c r="G169" s="7"/>
       <c r="H169" s="2"/>
       <c r="I169" s="2"/>
     </row>
     <row r="170" spans="1:9" ht="15">
       <c r="A170" s="8" t="s">
-        <v>97</v>
+        <v>509</v>
       </c>
       <c r="B170" s="4" t="s">
         <v>109</v>
@@ -4538,13 +4787,13 @@
         <v>24</v>
       </c>
       <c r="F170" s="2"/>
-      <c r="G170" s="2"/>
+      <c r="G170" s="7"/>
       <c r="H170" s="2"/>
       <c r="I170" s="2"/>
     </row>
     <row r="171" spans="1:9" ht="15">
       <c r="A171" s="6" t="s">
-        <v>114</v>
+        <v>510</v>
       </c>
       <c r="B171" s="6" t="s">
         <v>116</v>
@@ -4559,13 +4808,13 @@
         <v>38.6</v>
       </c>
       <c r="F171" s="2"/>
-      <c r="G171" s="2"/>
+      <c r="G171" s="7"/>
       <c r="H171" s="2"/>
       <c r="I171" s="2"/>
     </row>
     <row r="172" spans="1:9" ht="15">
       <c r="A172" s="6" t="s">
-        <v>118</v>
+        <v>511</v>
       </c>
       <c r="B172" s="6" t="s">
         <v>120</v>
@@ -4580,13 +4829,13 @@
         <v>26</v>
       </c>
       <c r="F172" s="2"/>
-      <c r="G172" s="2"/>
+      <c r="G172" s="7"/>
       <c r="H172" s="2"/>
       <c r="I172" s="2"/>
     </row>
     <row r="173" spans="1:9" ht="15">
       <c r="A173" s="6" t="s">
-        <v>122</v>
+        <v>512</v>
       </c>
       <c r="B173" s="6" t="s">
         <v>124</v>
@@ -4601,13 +4850,13 @@
         <v>10.8</v>
       </c>
       <c r="F173" s="2"/>
-      <c r="G173" s="2"/>
+      <c r="G173" s="7"/>
       <c r="H173" s="2"/>
       <c r="I173" s="2"/>
     </row>
     <row r="174" spans="1:9" ht="15">
       <c r="A174" s="6" t="s">
-        <v>126</v>
+        <v>513</v>
       </c>
       <c r="B174" s="6" t="s">
         <v>128</v>
@@ -4622,13 +4871,13 @@
         <v>31</v>
       </c>
       <c r="F174" s="2"/>
-      <c r="G174" s="2"/>
+      <c r="G174" s="7"/>
       <c r="H174" s="2"/>
       <c r="I174" s="2"/>
     </row>
     <row r="175" spans="1:9" ht="15">
       <c r="A175" s="6" t="s">
-        <v>130</v>
+        <v>514</v>
       </c>
       <c r="B175" s="6" t="s">
         <v>132</v>
@@ -4643,13 +4892,13 @@
         <v>34</v>
       </c>
       <c r="F175" s="2"/>
-      <c r="G175" s="2"/>
+      <c r="G175" s="7"/>
       <c r="H175" s="2"/>
       <c r="I175" s="2"/>
     </row>
     <row r="176" spans="1:9" ht="15">
       <c r="A176" s="6" t="s">
-        <v>134</v>
+        <v>515</v>
       </c>
       <c r="B176" s="6" t="s">
         <v>135</v>
@@ -4664,13 +4913,13 @@
         <v>53</v>
       </c>
       <c r="F176" s="2"/>
-      <c r="G176" s="2"/>
+      <c r="G176" s="7"/>
       <c r="H176" s="2"/>
       <c r="I176" s="2"/>
     </row>
     <row r="177" spans="1:9" ht="15">
       <c r="A177" s="6" t="s">
-        <v>138</v>
+        <v>516</v>
       </c>
       <c r="B177" s="6" t="s">
         <v>139</v>
@@ -4685,13 +4934,13 @@
         <v>47.3</v>
       </c>
       <c r="F177" s="2"/>
-      <c r="G177" s="2"/>
+      <c r="G177" s="7"/>
       <c r="H177" s="2"/>
       <c r="I177" s="2"/>
     </row>
     <row r="178" spans="1:9" ht="15">
       <c r="A178" s="6" t="s">
-        <v>141</v>
+        <v>517</v>
       </c>
       <c r="B178" s="6" t="s">
         <v>143</v>
@@ -4706,13 +4955,13 @@
         <v>26</v>
       </c>
       <c r="F178" s="2"/>
-      <c r="G178" s="2"/>
+      <c r="G178" s="7"/>
       <c r="H178" s="2"/>
       <c r="I178" s="2"/>
     </row>
     <row r="179" spans="1:9" ht="15">
       <c r="A179" s="6" t="s">
-        <v>145</v>
+        <v>518</v>
       </c>
       <c r="B179" s="6" t="s">
         <v>148</v>
@@ -4727,13 +4976,13 @@
         <v>33</v>
       </c>
       <c r="F179" s="2"/>
-      <c r="G179" s="2"/>
+      <c r="G179" s="7"/>
       <c r="H179" s="2"/>
       <c r="I179" s="2"/>
     </row>
     <row r="180" spans="1:9" ht="15">
       <c r="A180" s="6" t="s">
-        <v>150</v>
+        <v>519</v>
       </c>
       <c r="B180" s="6" t="s">
         <v>152</v>
@@ -4748,13 +4997,13 @@
         <v>14</v>
       </c>
       <c r="F180" s="2"/>
-      <c r="G180" s="2"/>
+      <c r="G180" s="7"/>
       <c r="H180" s="2"/>
       <c r="I180" s="2"/>
     </row>
     <row r="181" spans="1:9" ht="15">
       <c r="A181" s="6" t="s">
-        <v>154</v>
+        <v>520</v>
       </c>
       <c r="B181" s="6" t="s">
         <v>155</v>
@@ -4769,13 +5018,13 @@
         <v>19.3</v>
       </c>
       <c r="F181" s="2"/>
-      <c r="G181" s="2"/>
+      <c r="G181" s="7"/>
       <c r="H181" s="2"/>
       <c r="I181" s="2"/>
     </row>
     <row r="182" spans="1:9" ht="15">
       <c r="A182" s="6" t="s">
-        <v>158</v>
+        <v>521</v>
       </c>
       <c r="B182" s="6" t="s">
         <v>159</v>
@@ -4790,13 +5039,13 @@
         <v>81.099999999999994</v>
       </c>
       <c r="F182" s="2"/>
-      <c r="G182" s="2"/>
+      <c r="G182" s="7"/>
       <c r="H182" s="2"/>
       <c r="I182" s="2"/>
     </row>
     <row r="183" spans="1:9" ht="15">
       <c r="A183" s="6" t="s">
-        <v>162</v>
+        <v>522</v>
       </c>
       <c r="B183" s="6" t="s">
         <v>163</v>
@@ -4811,13 +5060,13 @@
         <v>34.299999999999997</v>
       </c>
       <c r="F183" s="2"/>
-      <c r="G183" s="2"/>
+      <c r="G183" s="7"/>
       <c r="H183" s="2"/>
       <c r="I183" s="2"/>
     </row>
     <row r="184" spans="1:9" ht="15">
       <c r="A184" s="6" t="s">
-        <v>164</v>
+        <v>523</v>
       </c>
       <c r="B184" s="6" t="s">
         <v>166</v>
@@ -4832,13 +5081,13 @@
         <v>57.8</v>
       </c>
       <c r="F184" s="2"/>
-      <c r="G184" s="2"/>
+      <c r="G184" s="7"/>
       <c r="H184" s="2"/>
       <c r="I184" s="2"/>
     </row>
     <row r="185" spans="1:9" ht="15">
       <c r="A185" s="6" t="s">
-        <v>168</v>
+        <v>524</v>
       </c>
       <c r="B185" s="6" t="s">
         <v>170</v>
@@ -4853,13 +5102,13 @@
         <v>34</v>
       </c>
       <c r="F185" s="2"/>
-      <c r="G185" s="2"/>
+      <c r="G185" s="7"/>
       <c r="H185" s="2"/>
       <c r="I185" s="2"/>
     </row>
     <row r="186" spans="1:9" ht="15">
       <c r="A186" s="6" t="s">
-        <v>171</v>
+        <v>491</v>
       </c>
       <c r="B186" s="6" t="s">
         <v>173</v>
@@ -4874,13 +5123,13 @@
         <v>21</v>
       </c>
       <c r="F186" s="2"/>
-      <c r="G186" s="2"/>
+      <c r="G186" s="7"/>
       <c r="H186" s="2"/>
       <c r="I186" s="2"/>
     </row>
     <row r="187" spans="1:9" ht="15">
       <c r="A187" s="6" t="s">
-        <v>174</v>
+        <v>525</v>
       </c>
       <c r="B187" s="6" t="s">
         <v>175</v>
@@ -4895,13 +5144,13 @@
         <v>47.9</v>
       </c>
       <c r="F187" s="2"/>
-      <c r="G187" s="2"/>
+      <c r="G187" s="7"/>
       <c r="H187" s="2"/>
       <c r="I187" s="2"/>
     </row>
     <row r="188" spans="1:9" ht="15">
       <c r="A188" s="6" t="s">
-        <v>176</v>
+        <v>526</v>
       </c>
       <c r="B188" s="6" t="s">
         <v>177</v>
@@ -4916,13 +5165,13 @@
         <v>69.2</v>
       </c>
       <c r="F188" s="2"/>
-      <c r="G188" s="2"/>
+      <c r="G188" s="7"/>
       <c r="H188" s="2"/>
       <c r="I188" s="2"/>
     </row>
     <row r="189" spans="1:9" ht="15">
       <c r="A189" s="6" t="s">
-        <v>179</v>
+        <v>527</v>
       </c>
       <c r="B189" s="6" t="s">
         <v>180</v>
@@ -4937,13 +5186,13 @@
         <v>91.6</v>
       </c>
       <c r="F189" s="2"/>
-      <c r="G189" s="2"/>
+      <c r="G189" s="7"/>
       <c r="H189" s="2"/>
       <c r="I189" s="2"/>
     </row>
     <row r="190" spans="1:9" ht="15">
       <c r="A190" s="6" t="s">
-        <v>181</v>
+        <v>528</v>
       </c>
       <c r="B190" s="6" t="s">
         <v>183</v>
@@ -4958,13 +5207,13 @@
         <v>31</v>
       </c>
       <c r="F190" s="2"/>
-      <c r="G190" s="2"/>
+      <c r="G190" s="7"/>
       <c r="H190" s="2"/>
       <c r="I190" s="2"/>
     </row>
     <row r="191" spans="1:9" ht="15">
       <c r="A191" s="6" t="s">
-        <v>190</v>
+        <v>529</v>
       </c>
       <c r="B191" s="6" t="s">
         <v>192</v>
@@ -4979,13 +5228,13 @@
         <v>34</v>
       </c>
       <c r="F191" s="2"/>
-      <c r="G191" s="2"/>
+      <c r="G191" s="7"/>
       <c r="H191" s="2"/>
       <c r="I191" s="2"/>
     </row>
     <row r="192" spans="1:9" ht="15">
       <c r="A192" s="6" t="s">
-        <v>193</v>
+        <v>530</v>
       </c>
       <c r="B192" s="6" t="s">
         <v>194</v>
@@ -5000,13 +5249,13 @@
         <v>20</v>
       </c>
       <c r="F192" s="2"/>
-      <c r="G192" s="2"/>
+      <c r="G192" s="7"/>
       <c r="H192" s="2"/>
       <c r="I192" s="2"/>
     </row>
     <row r="193" spans="1:9" ht="15">
       <c r="A193" s="6" t="s">
-        <v>195</v>
+        <v>531</v>
       </c>
       <c r="B193" s="6" t="s">
         <v>196</v>
@@ -5021,13 +5270,13 @@
         <v>41</v>
       </c>
       <c r="F193" s="2"/>
-      <c r="G193" s="2"/>
+      <c r="G193" s="7"/>
       <c r="H193" s="2"/>
       <c r="I193" s="2"/>
     </row>
     <row r="194" spans="1:9" ht="15">
       <c r="A194" s="6" t="s">
-        <v>198</v>
+        <v>532</v>
       </c>
       <c r="B194" s="6" t="s">
         <v>199</v>
@@ -5042,13 +5291,13 @@
         <v>30</v>
       </c>
       <c r="F194" s="2"/>
-      <c r="G194" s="2"/>
+      <c r="G194" s="7"/>
       <c r="H194" s="2"/>
       <c r="I194" s="2"/>
     </row>
     <row r="195" spans="1:9" ht="15">
       <c r="A195" s="6" t="s">
-        <v>201</v>
+        <v>533</v>
       </c>
       <c r="B195" s="6" t="s">
         <v>203</v>
@@ -5063,13 +5312,13 @@
         <v>36</v>
       </c>
       <c r="F195" s="2"/>
-      <c r="G195" s="2"/>
+      <c r="G195" s="7"/>
       <c r="H195" s="2"/>
       <c r="I195" s="2"/>
     </row>
     <row r="196" spans="1:9" ht="15">
       <c r="A196" s="6" t="s">
-        <v>205</v>
+        <v>534</v>
       </c>
       <c r="B196" s="6" t="s">
         <v>207</v>
@@ -5084,13 +5333,13 @@
         <v>13</v>
       </c>
       <c r="F196" s="2"/>
-      <c r="G196" s="2"/>
+      <c r="G196" s="7"/>
       <c r="H196" s="2"/>
       <c r="I196" s="2"/>
     </row>
     <row r="197" spans="1:9" ht="15">
       <c r="A197" s="6" t="s">
-        <v>209</v>
+        <v>535</v>
       </c>
       <c r="B197" s="6" t="s">
         <v>211</v>
@@ -5105,13 +5354,13 @@
         <v>55</v>
       </c>
       <c r="F197" s="2"/>
-      <c r="G197" s="2"/>
+      <c r="G197" s="7"/>
       <c r="H197" s="2"/>
       <c r="I197" s="2"/>
     </row>
     <row r="198" spans="1:9" ht="15">
       <c r="A198" s="6" t="s">
-        <v>213</v>
+        <v>536</v>
       </c>
       <c r="B198" s="6" t="s">
         <v>215</v>
@@ -5126,13 +5375,13 @@
         <v>36</v>
       </c>
       <c r="F198" s="2"/>
-      <c r="G198" s="2"/>
+      <c r="G198" s="7"/>
       <c r="H198" s="2"/>
       <c r="I198" s="2"/>
     </row>
     <row r="199" spans="1:9" ht="15">
       <c r="A199" s="6" t="s">
-        <v>216</v>
+        <v>537</v>
       </c>
       <c r="B199" s="6" t="s">
         <v>218</v>
@@ -5147,13 +5396,13 @@
         <v>58</v>
       </c>
       <c r="F199" s="2"/>
-      <c r="G199" s="2"/>
+      <c r="G199" s="7"/>
       <c r="H199" s="2"/>
       <c r="I199" s="2"/>
     </row>
     <row r="200" spans="1:9" ht="15">
       <c r="A200" s="6" t="s">
-        <v>220</v>
+        <v>538</v>
       </c>
       <c r="B200" s="6" t="s">
         <v>221</v>
@@ -5168,13 +5417,13 @@
         <v>30</v>
       </c>
       <c r="F200" s="2"/>
-      <c r="G200" s="2"/>
+      <c r="G200" s="7"/>
       <c r="H200" s="2"/>
       <c r="I200" s="2"/>
     </row>
     <row r="201" spans="1:9" ht="15">
       <c r="A201" s="6" t="s">
-        <v>224</v>
+        <v>539</v>
       </c>
       <c r="B201" s="6" t="s">
         <v>225</v>
@@ -5189,13 +5438,13 @@
         <v>32</v>
       </c>
       <c r="F201" s="2"/>
-      <c r="G201" s="2"/>
+      <c r="G201" s="7"/>
       <c r="H201" s="2"/>
       <c r="I201" s="2"/>
     </row>
     <row r="202" spans="1:9" ht="15">
       <c r="A202" s="6" t="s">
-        <v>227</v>
+        <v>540</v>
       </c>
       <c r="B202" s="6" t="s">
         <v>228</v>
@@ -5210,13 +5459,13 @@
         <v>13</v>
       </c>
       <c r="F202" s="2"/>
-      <c r="G202" s="2"/>
+      <c r="G202" s="7"/>
       <c r="H202" s="2"/>
       <c r="I202" s="2"/>
     </row>
     <row r="203" spans="1:9" ht="15">
       <c r="A203" s="6" t="s">
-        <v>231</v>
+        <v>541</v>
       </c>
       <c r="B203" s="6" t="s">
         <v>232</v>
@@ -5231,13 +5480,13 @@
         <v>15</v>
       </c>
       <c r="F203" s="2"/>
-      <c r="G203" s="2"/>
+      <c r="G203" s="7"/>
       <c r="H203" s="2"/>
       <c r="I203" s="2"/>
     </row>
     <row r="204" spans="1:9" ht="15">
       <c r="A204" s="6" t="s">
-        <v>234</v>
+        <v>542</v>
       </c>
       <c r="B204" s="6" t="s">
         <v>236</v>
@@ -5252,13 +5501,13 @@
         <v>34</v>
       </c>
       <c r="F204" s="2"/>
-      <c r="G204" s="2"/>
+      <c r="G204" s="7"/>
       <c r="H204" s="2"/>
       <c r="I204" s="2"/>
     </row>
     <row r="205" spans="1:9" ht="15">
       <c r="A205" s="6" t="s">
-        <v>238</v>
+        <v>543</v>
       </c>
       <c r="B205" s="6" t="s">
         <v>240</v>
@@ -5273,13 +5522,13 @@
         <v>22</v>
       </c>
       <c r="F205" s="2"/>
-      <c r="G205" s="2"/>
+      <c r="G205" s="7"/>
       <c r="H205" s="2"/>
       <c r="I205" s="2"/>
     </row>
     <row r="206" spans="1:9" ht="15">
       <c r="A206" s="6" t="s">
-        <v>242</v>
+        <v>544</v>
       </c>
       <c r="B206" s="6" t="s">
         <v>244</v>
@@ -5294,13 +5543,13 @@
         <v>48</v>
       </c>
       <c r="F206" s="2"/>
-      <c r="G206" s="2"/>
+      <c r="G206" s="7"/>
       <c r="H206" s="2"/>
       <c r="I206" s="2"/>
     </row>
     <row r="207" spans="1:9" ht="15">
       <c r="A207" s="6" t="s">
-        <v>246</v>
+        <v>545</v>
       </c>
       <c r="B207" s="6" t="s">
         <v>248</v>
@@ -5315,13 +5564,13 @@
         <v>31</v>
       </c>
       <c r="F207" s="2"/>
-      <c r="G207" s="2"/>
+      <c r="G207" s="7"/>
       <c r="H207" s="2"/>
       <c r="I207" s="2"/>
     </row>
     <row r="208" spans="1:9" ht="15">
       <c r="A208" s="6" t="s">
-        <v>250</v>
+        <v>546</v>
       </c>
       <c r="B208" s="6" t="s">
         <v>252</v>
@@ -5336,13 +5585,13 @@
         <v>24</v>
       </c>
       <c r="F208" s="2"/>
-      <c r="G208" s="2"/>
+      <c r="G208" s="7"/>
       <c r="H208" s="2"/>
       <c r="I208" s="2"/>
     </row>
     <row r="209" spans="1:9" ht="15">
       <c r="A209" s="6" t="s">
-        <v>253</v>
+        <v>419</v>
       </c>
       <c r="B209" s="6" t="s">
         <v>255</v>
@@ -5357,13 +5606,13 @@
         <v>54</v>
       </c>
       <c r="F209" s="2"/>
-      <c r="G209" s="2"/>
+      <c r="G209" s="7"/>
       <c r="H209" s="2"/>
       <c r="I209" s="2"/>
     </row>
     <row r="210" spans="1:9" ht="15">
       <c r="A210" s="6" t="s">
-        <v>257</v>
+        <v>421</v>
       </c>
       <c r="B210" s="6" t="s">
         <v>259</v>
@@ -5378,13 +5627,13 @@
         <v>46</v>
       </c>
       <c r="F210" s="2"/>
-      <c r="G210" s="2"/>
+      <c r="G210" s="7"/>
       <c r="H210" s="2"/>
       <c r="I210" s="2"/>
     </row>
     <row r="211" spans="1:9" ht="15">
       <c r="A211" s="6" t="s">
-        <v>261</v>
+        <v>423</v>
       </c>
       <c r="B211" s="6" t="s">
         <v>263</v>
@@ -5399,13 +5648,13 @@
         <v>38</v>
       </c>
       <c r="F211" s="2"/>
-      <c r="G211" s="2"/>
+      <c r="G211" s="7"/>
       <c r="H211" s="2"/>
       <c r="I211" s="2"/>
     </row>
     <row r="212" spans="1:9" ht="15">
       <c r="A212" s="6" t="s">
-        <v>265</v>
+        <v>547</v>
       </c>
       <c r="B212" s="6" t="s">
         <v>266</v>
@@ -5420,13 +5669,13 @@
         <v>47</v>
       </c>
       <c r="F212" s="2"/>
-      <c r="G212" s="2"/>
+      <c r="G212" s="7"/>
       <c r="H212" s="2"/>
       <c r="I212" s="2"/>
     </row>
     <row r="213" spans="1:9" ht="15">
       <c r="A213" s="6" t="s">
-        <v>269</v>
+        <v>427</v>
       </c>
       <c r="B213" s="6" t="s">
         <v>270</v>
@@ -5441,13 +5690,13 @@
         <v>47</v>
       </c>
       <c r="F213" s="2"/>
-      <c r="G213" s="2"/>
+      <c r="G213" s="7"/>
       <c r="H213" s="2"/>
       <c r="I213" s="2"/>
     </row>
     <row r="214" spans="1:9" ht="15">
       <c r="A214" s="6" t="s">
-        <v>273</v>
+        <v>429</v>
       </c>
       <c r="B214" s="6" t="s">
         <v>274</v>
@@ -5462,13 +5711,13 @@
         <v>45</v>
       </c>
       <c r="F214" s="2"/>
-      <c r="G214" s="2"/>
+      <c r="G214" s="7"/>
       <c r="H214" s="2"/>
       <c r="I214" s="2"/>
     </row>
     <row r="215" spans="1:9" ht="15">
       <c r="A215" s="6" t="s">
-        <v>277</v>
+        <v>431</v>
       </c>
       <c r="B215" s="6" t="s">
         <v>278</v>
@@ -5483,13 +5732,13 @@
         <v>36</v>
       </c>
       <c r="F215" s="2"/>
-      <c r="G215" s="2"/>
+      <c r="G215" s="7"/>
       <c r="H215" s="2"/>
       <c r="I215" s="2"/>
     </row>
     <row r="216" spans="1:9" ht="15">
       <c r="A216" s="6" t="s">
-        <v>281</v>
+        <v>433</v>
       </c>
       <c r="B216" s="6" t="s">
         <v>282</v>
@@ -5504,13 +5753,13 @@
         <v>46</v>
       </c>
       <c r="F216" s="2"/>
-      <c r="G216" s="2"/>
+      <c r="G216" s="7"/>
       <c r="H216" s="2"/>
       <c r="I216" s="2"/>
     </row>
     <row r="217" spans="1:9" ht="15">
       <c r="A217" s="6" t="s">
-        <v>285</v>
+        <v>435</v>
       </c>
       <c r="B217" s="6" t="s">
         <v>286</v>
@@ -5525,13 +5774,13 @@
         <v>52</v>
       </c>
       <c r="F217" s="2"/>
-      <c r="G217" s="2"/>
+      <c r="G217" s="7"/>
       <c r="H217" s="2"/>
       <c r="I217" s="2"/>
     </row>
     <row r="218" spans="1:9" ht="15">
       <c r="A218" s="6" t="s">
-        <v>289</v>
+        <v>548</v>
       </c>
       <c r="B218" s="6" t="s">
         <v>290</v>
@@ -5546,13 +5795,13 @@
         <v>34</v>
       </c>
       <c r="F218" s="2"/>
-      <c r="G218" s="2"/>
+      <c r="G218" s="7"/>
       <c r="H218" s="2"/>
       <c r="I218" s="2"/>
     </row>
     <row r="219" spans="1:9" ht="15">
       <c r="A219" s="6" t="s">
-        <v>293</v>
+        <v>439</v>
       </c>
       <c r="B219" s="6" t="s">
         <v>294</v>
@@ -5567,13 +5816,13 @@
         <v>32</v>
       </c>
       <c r="F219" s="2"/>
-      <c r="G219" s="2"/>
+      <c r="G219" s="7"/>
       <c r="H219" s="2"/>
       <c r="I219" s="2"/>
     </row>
     <row r="220" spans="1:9" ht="15">
       <c r="A220" s="6" t="s">
-        <v>296</v>
+        <v>441</v>
       </c>
       <c r="B220" s="6" t="s">
         <v>298</v>
@@ -5588,13 +5837,13 @@
         <v>33</v>
       </c>
       <c r="F220" s="2"/>
-      <c r="G220" s="2"/>
+      <c r="G220" s="7"/>
       <c r="H220" s="2"/>
       <c r="I220" s="2"/>
     </row>
     <row r="221" spans="1:9" ht="15">
       <c r="A221" s="6" t="s">
-        <v>300</v>
+        <v>443</v>
       </c>
       <c r="B221" s="6" t="s">
         <v>302</v>
@@ -5609,13 +5858,13 @@
         <v>39</v>
       </c>
       <c r="F221" s="2"/>
-      <c r="G221" s="2"/>
+      <c r="G221" s="7"/>
       <c r="H221" s="2"/>
       <c r="I221" s="2"/>
     </row>
     <row r="222" spans="1:9" ht="15">
       <c r="A222" s="6" t="s">
-        <v>304</v>
+        <v>445</v>
       </c>
       <c r="B222" s="6" t="s">
         <v>305</v>
@@ -5630,13 +5879,13 @@
         <v>59</v>
       </c>
       <c r="F222" s="2"/>
-      <c r="G222" s="2"/>
+      <c r="G222" s="7"/>
       <c r="H222" s="2"/>
       <c r="I222" s="2"/>
     </row>
     <row r="223" spans="1:9" ht="15">
       <c r="A223" s="6" t="s">
-        <v>307</v>
+        <v>447</v>
       </c>
       <c r="B223" s="6" t="s">
         <v>308</v>
@@ -5651,13 +5900,13 @@
         <v>19</v>
       </c>
       <c r="F223" s="2"/>
-      <c r="G223" s="2"/>
+      <c r="G223" s="7"/>
       <c r="H223" s="2"/>
       <c r="I223" s="2"/>
     </row>
     <row r="224" spans="1:9" ht="15">
       <c r="A224" s="6" t="s">
-        <v>310</v>
+        <v>451</v>
       </c>
       <c r="B224" s="6" t="s">
         <v>312</v>
@@ -5672,13 +5921,13 @@
         <v>59</v>
       </c>
       <c r="F224" s="2"/>
-      <c r="G224" s="2"/>
+      <c r="G224" s="7"/>
       <c r="H224" s="2"/>
       <c r="I224" s="2"/>
     </row>
     <row r="225" spans="1:9" ht="15">
       <c r="A225" s="6" t="s">
-        <v>313</v>
+        <v>549</v>
       </c>
       <c r="B225" s="6" t="s">
         <v>314</v>
@@ -5693,13 +5942,13 @@
         <v>74</v>
       </c>
       <c r="F225" s="2"/>
-      <c r="G225" s="2"/>
+      <c r="G225" s="7"/>
       <c r="H225" s="2"/>
       <c r="I225" s="2"/>
     </row>
     <row r="226" spans="1:9" ht="15">
       <c r="A226" s="6" t="s">
-        <v>316</v>
+        <v>455</v>
       </c>
       <c r="B226" s="6" t="s">
         <v>317</v>
@@ -5714,13 +5963,13 @@
         <v>62</v>
       </c>
       <c r="F226" s="2"/>
-      <c r="G226" s="2"/>
+      <c r="G226" s="7"/>
       <c r="H226" s="2"/>
       <c r="I226" s="2"/>
     </row>
     <row r="227" spans="1:9" ht="15">
       <c r="A227" s="6" t="s">
-        <v>319</v>
+        <v>457</v>
       </c>
       <c r="B227" s="6" t="s">
         <v>321</v>
@@ -5735,13 +5984,13 @@
         <v>47</v>
       </c>
       <c r="F227" s="2"/>
-      <c r="G227" s="2"/>
+      <c r="G227" s="7"/>
       <c r="H227" s="2"/>
       <c r="I227" s="2"/>
     </row>
     <row r="228" spans="1:9" ht="15">
       <c r="A228" s="6" t="s">
-        <v>323</v>
+        <v>550</v>
       </c>
       <c r="B228" s="6" t="s">
         <v>325</v>
@@ -5756,13 +6005,13 @@
         <v>14</v>
       </c>
       <c r="F228" s="2"/>
-      <c r="G228" s="2"/>
+      <c r="G228" s="7"/>
       <c r="H228" s="2"/>
       <c r="I228" s="2"/>
     </row>
     <row r="229" spans="1:9" ht="15">
       <c r="A229" s="6" t="s">
-        <v>327</v>
+        <v>551</v>
       </c>
       <c r="B229" s="6" t="s">
         <v>329</v>
@@ -5777,13 +6026,13 @@
         <v>20</v>
       </c>
       <c r="F229" s="2"/>
-      <c r="G229" s="2"/>
+      <c r="G229" s="7"/>
       <c r="H229" s="2"/>
       <c r="I229" s="2"/>
     </row>
     <row r="230" spans="1:9" ht="15">
       <c r="A230" s="6" t="s">
-        <v>331</v>
+        <v>552</v>
       </c>
       <c r="B230" s="6" t="s">
         <v>333</v>
@@ -5798,13 +6047,13 @@
         <v>18</v>
       </c>
       <c r="F230" s="2"/>
-      <c r="G230" s="2"/>
+      <c r="G230" s="7"/>
       <c r="H230" s="2"/>
       <c r="I230" s="2"/>
     </row>
     <row r="231" spans="1:9" ht="15">
       <c r="A231" s="6" t="s">
-        <v>335</v>
+        <v>553</v>
       </c>
       <c r="B231" s="6" t="s">
         <v>337</v>
@@ -5819,13 +6068,13 @@
         <v>7</v>
       </c>
       <c r="F231" s="2"/>
-      <c r="G231" s="2"/>
+      <c r="G231" s="7"/>
       <c r="H231" s="2"/>
       <c r="I231" s="2"/>
     </row>
     <row r="232" spans="1:9" ht="15">
       <c r="A232" s="6" t="s">
-        <v>338</v>
+        <v>554</v>
       </c>
       <c r="B232" s="6" t="s">
         <v>340</v>
@@ -5840,13 +6089,13 @@
         <v>38</v>
       </c>
       <c r="F232" s="2"/>
-      <c r="G232" s="2"/>
+      <c r="G232" s="7"/>
       <c r="H232" s="2"/>
       <c r="I232" s="2"/>
     </row>
     <row r="233" spans="1:9" ht="15">
       <c r="A233" s="6" t="s">
-        <v>342</v>
+        <v>555</v>
       </c>
       <c r="B233" s="6" t="s">
         <v>344</v>
@@ -5861,13 +6110,13 @@
         <v>38</v>
       </c>
       <c r="F233" s="2"/>
-      <c r="G233" s="2"/>
+      <c r="G233" s="7"/>
       <c r="H233" s="2"/>
       <c r="I233" s="2"/>
     </row>
     <row r="234" spans="1:9" ht="15">
       <c r="A234" s="6" t="s">
-        <v>346</v>
+        <v>532</v>
       </c>
       <c r="B234" s="6" t="s">
         <v>348</v>
@@ -5882,13 +6131,13 @@
         <v>21</v>
       </c>
       <c r="F234" s="2"/>
-      <c r="G234" s="2"/>
+      <c r="G234" s="7"/>
       <c r="H234" s="2"/>
       <c r="I234" s="2"/>
     </row>
     <row r="235" spans="1:9" ht="15">
       <c r="A235" s="6" t="s">
-        <v>357</v>
+        <v>556</v>
       </c>
       <c r="B235" s="6" t="s">
         <v>359</v>
@@ -5903,13 +6152,13 @@
         <v>31</v>
       </c>
       <c r="F235" s="2"/>
-      <c r="G235" s="2"/>
+      <c r="G235" s="7"/>
       <c r="H235" s="2"/>
       <c r="I235" s="2"/>
     </row>
     <row r="236" spans="1:9" ht="15">
       <c r="A236" s="6" t="s">
-        <v>360</v>
+        <v>557</v>
       </c>
       <c r="B236" s="6" t="s">
         <v>362</v>
@@ -5924,13 +6173,13 @@
         <v>71</v>
       </c>
       <c r="F236" s="2"/>
-      <c r="G236" s="2"/>
+      <c r="G236" s="7"/>
       <c r="H236" s="2"/>
       <c r="I236" s="2"/>
     </row>
     <row r="237" spans="1:9" ht="15">
       <c r="A237" s="6" t="s">
-        <v>364</v>
+        <v>558</v>
       </c>
       <c r="B237" s="6" t="s">
         <v>365</v>
@@ -5945,13 +6194,13 @@
         <v>22</v>
       </c>
       <c r="F237" s="2"/>
-      <c r="G237" s="2"/>
+      <c r="G237" s="7"/>
       <c r="H237" s="2"/>
       <c r="I237" s="2"/>
     </row>
     <row r="238" spans="1:9" ht="15">
       <c r="A238" s="6" t="s">
-        <v>368</v>
+        <v>559</v>
       </c>
       <c r="B238" s="6" t="s">
         <v>369</v>
@@ -5966,13 +6215,13 @@
         <v>42</v>
       </c>
       <c r="F238" s="2"/>
-      <c r="G238" s="2"/>
+      <c r="G238" s="7"/>
       <c r="H238" s="2"/>
       <c r="I238" s="2"/>
     </row>
     <row r="239" spans="1:9" ht="15">
       <c r="A239" s="6" t="s">
-        <v>372</v>
+        <v>560</v>
       </c>
       <c r="B239" s="6" t="s">
         <v>375</v>
@@ -5987,13 +6236,13 @@
         <v>4</v>
       </c>
       <c r="F239" s="2"/>
-      <c r="G239" s="2"/>
+      <c r="G239" s="7"/>
       <c r="H239" s="2"/>
       <c r="I239" s="2"/>
     </row>
     <row r="240" spans="1:9" ht="15">
       <c r="A240" s="6" t="s">
-        <v>377</v>
+        <v>561</v>
       </c>
       <c r="B240" s="6" t="s">
         <v>379</v>
@@ -6008,13 +6257,13 @@
         <v>27</v>
       </c>
       <c r="F240" s="2"/>
-      <c r="G240" s="2"/>
+      <c r="G240" s="7"/>
       <c r="H240" s="2"/>
       <c r="I240" s="2"/>
     </row>
     <row r="241" spans="1:9" ht="15">
       <c r="A241" s="6" t="s">
-        <v>380</v>
+        <v>562</v>
       </c>
       <c r="B241" s="6" t="s">
         <v>382</v>
@@ -6029,13 +6278,13 @@
         <v>24</v>
       </c>
       <c r="F241" s="2"/>
-      <c r="G241" s="2"/>
+      <c r="G241" s="7"/>
       <c r="H241" s="2"/>
       <c r="I241" s="2"/>
     </row>
     <row r="242" spans="1:9" ht="15">
       <c r="A242" s="6" t="s">
-        <v>383</v>
+        <v>563</v>
       </c>
       <c r="B242" s="6" t="s">
         <v>386</v>
@@ -6050,13 +6299,13 @@
         <v>32</v>
       </c>
       <c r="F242" s="2"/>
-      <c r="G242" s="2"/>
+      <c r="G242" s="7"/>
       <c r="H242" s="2"/>
       <c r="I242" s="2"/>
     </row>
     <row r="243" spans="1:9" ht="15">
       <c r="A243" s="6" t="s">
-        <v>387</v>
+        <v>564</v>
       </c>
       <c r="B243" s="6" t="s">
         <v>388</v>
@@ -6071,13 +6320,13 @@
         <v>61</v>
       </c>
       <c r="F243" s="2"/>
-      <c r="G243" s="2"/>
+      <c r="G243" s="7"/>
       <c r="H243" s="2"/>
       <c r="I243" s="2"/>
     </row>
     <row r="244" spans="1:9" ht="15">
       <c r="A244" s="6" t="s">
-        <v>389</v>
+        <v>565</v>
       </c>
       <c r="B244" s="6" t="s">
         <v>390</v>
@@ -6092,13 +6341,13 @@
         <v>49</v>
       </c>
       <c r="F244" s="2"/>
-      <c r="G244" s="2"/>
+      <c r="G244" s="7"/>
       <c r="H244" s="2"/>
       <c r="I244" s="2"/>
     </row>
     <row r="245" spans="1:9" ht="15">
       <c r="A245" s="6" t="s">
-        <v>391</v>
+        <v>566</v>
       </c>
       <c r="B245" s="6" t="s">
         <v>393</v>
@@ -6113,13 +6362,13 @@
         <v>46.8</v>
       </c>
       <c r="F245" s="2"/>
-      <c r="G245" s="2"/>
+      <c r="G245" s="7"/>
       <c r="H245" s="2"/>
       <c r="I245" s="2"/>
     </row>
     <row r="246" spans="1:9" ht="15">
       <c r="A246" s="6" t="s">
-        <v>395</v>
+        <v>567</v>
       </c>
       <c r="B246" s="6" t="s">
         <v>396</v>
@@ -6134,13 +6383,13 @@
         <v>79.5</v>
       </c>
       <c r="F246" s="2"/>
-      <c r="G246" s="2"/>
+      <c r="G246" s="7"/>
       <c r="H246" s="2"/>
       <c r="I246" s="2"/>
     </row>
     <row r="247" spans="1:9" ht="15">
       <c r="A247" s="6" t="s">
-        <v>399</v>
+        <v>568</v>
       </c>
       <c r="B247" s="6" t="s">
         <v>400</v>
@@ -6155,13 +6404,13 @@
         <v>25</v>
       </c>
       <c r="F247" s="2"/>
-      <c r="G247" s="2"/>
+      <c r="G247" s="7"/>
       <c r="H247" s="2"/>
       <c r="I247" s="2"/>
     </row>
     <row r="248" spans="1:9" ht="15">
       <c r="A248" s="6" t="s">
-        <v>402</v>
+        <v>569</v>
       </c>
       <c r="B248" s="6" t="s">
         <v>404</v>
@@ -6176,13 +6425,13 @@
         <v>21.3</v>
       </c>
       <c r="F248" s="2"/>
-      <c r="G248" s="2"/>
+      <c r="G248" s="7"/>
       <c r="H248" s="2"/>
       <c r="I248" s="2"/>
     </row>
     <row r="249" spans="1:9" ht="15">
       <c r="A249" s="6" t="s">
-        <v>405</v>
+        <v>570</v>
       </c>
       <c r="B249" s="6" t="s">
         <v>407</v>
@@ -6197,13 +6446,13 @@
         <v>58.3</v>
       </c>
       <c r="F249" s="2"/>
-      <c r="G249" s="2"/>
+      <c r="G249" s="7"/>
       <c r="H249" s="2"/>
       <c r="I249" s="2"/>
     </row>
     <row r="250" spans="1:9" ht="15">
       <c r="A250" s="6" t="s">
-        <v>408</v>
+        <v>571</v>
       </c>
       <c r="B250" s="6" t="s">
         <v>409</v>
@@ -6218,13 +6467,13 @@
         <v>35.5</v>
       </c>
       <c r="F250" s="2"/>
-      <c r="G250" s="2"/>
+      <c r="G250" s="7"/>
       <c r="H250" s="2"/>
       <c r="I250" s="2"/>
     </row>
     <row r="251" spans="1:9" ht="15">
       <c r="A251" s="6" t="s">
-        <v>412</v>
+        <v>572</v>
       </c>
       <c r="B251" s="6" t="s">
         <v>413</v>
@@ -6239,7 +6488,7 @@
         <v>30</v>
       </c>
       <c r="F251" s="2"/>
-      <c r="G251" s="2"/>
+      <c r="G251" s="7"/>
       <c r="H251" s="2"/>
       <c r="I251" s="2"/>
     </row>
@@ -6249,7 +6498,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -6257,12 +6506,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="61.85546875" customWidth="1"/>
-    <col min="2" max="2" width="22.28515625" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" customWidth="1"/>
+    <col min="1" max="1" width="61.83203125" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" customWidth="1"/>
+    <col min="3" max="3" width="18.83203125" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">

</xml_diff>